<commit_message>
imputation procedure and data sets
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="16440"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="15960" windowHeight="16380"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -70,17 +70,6 @@
         <rFont val="Verdana"/>
         <family val="2"/>
       </rPr>
-      <t>Are you left-handed?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
       <t>Do you live alone?</t>
     </r>
   </si>
@@ -180,17 +169,6 @@
         <rFont val="Verdana"/>
         <family val="2"/>
       </rPr>
-      <t>Do you eat breakfast every day?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
       <t>Are you currently carrying a grudge against anyone in your personal life?</t>
     </r>
   </si>
@@ -334,17 +312,6 @@
         <rFont val="Verdana"/>
         <family val="2"/>
       </rPr>
-      <t>Lots of people are around! Are you more likely to be right in the middle of things, or looking for your own quieter space?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
       <t>Are you generally a cautious person, or are you comfortable taking risks?</t>
     </r>
   </si>
@@ -378,17 +345,6 @@
         <rFont val="Verdana"/>
         <family val="2"/>
       </rPr>
-      <t>Is your alarm clock intentionally set to be a few minutes fast?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
       <t>As a teenager, do/did you have parents who were generally more supportive or demanding?</t>
     </r>
   </si>
@@ -587,17 +543,6 @@
         <rFont val="Verdana"/>
         <family val="2"/>
       </rPr>
-      <t>Do you find it easier to start and maintain a new good habit, or to permanently kick a bad habit?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
       <t>Are you a morning person or a night person?</t>
     </r>
   </si>
@@ -1375,6 +1320,21 @@
   </si>
   <si>
     <t>Do you own any power tools? (power saws, drills, etc.)</t>
+  </si>
+  <si>
+    <t>Do you find it easier to start and maintain a new good habit, or to permanently kick a bad habit?</t>
+  </si>
+  <si>
+    <t>Is your alarm clock intentionally set to be a few minutes fast?</t>
+  </si>
+  <si>
+    <t>Are you left-handed?</t>
+  </si>
+  <si>
+    <t>Do you eat breakfast every day?</t>
+  </si>
+  <si>
+    <t>Lots of people are around! Are you more likely to be right in the middle of things, or looking for your own quieter space?</t>
   </si>
 </sst>
 </file>
@@ -2882,8 +2842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2898,19 +2858,19 @@
   <sheetData>
     <row r="1" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2918,13 +2878,13 @@
         <v>124742</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E2">
         <v>101</v>
@@ -2935,13 +2895,13 @@
         <v>124122</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -2952,13 +2912,13 @@
         <v>123621</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E4" s="20">
         <v>99</v>
@@ -3221,13 +3181,13 @@
         <v>123464</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="E5">
         <v>98</v>
@@ -3238,13 +3198,13 @@
         <v>122771</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E6">
         <v>97</v>
@@ -3255,13 +3215,13 @@
         <v>122770</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E7">
         <v>96</v>
@@ -3272,13 +3232,13 @@
         <v>122769</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E8">
         <v>95</v>
@@ -3289,13 +3249,13 @@
         <v>122120</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E9">
         <v>94</v>
@@ -3306,13 +3266,13 @@
         <v>121700</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E10">
         <v>93</v>
@@ -3323,13 +3283,13 @@
         <v>121699</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E11">
         <v>92</v>
@@ -3340,13 +3300,13 @@
         <v>121011</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E12">
         <v>91</v>
@@ -3357,13 +3317,13 @@
         <v>120978</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E13">
         <v>90</v>
@@ -3374,13 +3334,13 @@
         <v>120650</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E14">
         <v>89</v>
@@ -3391,13 +3351,13 @@
         <v>120472</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E15" s="39">
         <v>88</v>
@@ -3660,13 +3620,13 @@
         <v>120379</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E16" s="39">
         <v>87</v>
@@ -3929,13 +3889,13 @@
         <v>120194</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E17">
         <v>86</v>
@@ -3946,13 +3906,13 @@
         <v>120014</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E18">
         <v>85</v>
@@ -3963,13 +3923,13 @@
         <v>120012</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E19">
         <v>84</v>
@@ -3980,13 +3940,13 @@
         <v>119851</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E20">
         <v>83</v>
@@ -3997,13 +3957,13 @@
         <v>119650</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E21">
         <v>82</v>
@@ -4014,13 +3974,13 @@
         <v>119334</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E22">
         <v>81</v>
@@ -4031,13 +3991,13 @@
         <v>118892</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E23">
         <v>80</v>
@@ -4048,13 +4008,13 @@
         <v>118237</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E24">
         <v>79</v>
@@ -4065,13 +4025,13 @@
         <v>118233</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E25">
         <v>78</v>
@@ -4082,13 +4042,13 @@
         <v>118232</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E26">
         <v>77</v>
@@ -4099,13 +4059,13 @@
         <v>118117</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E27">
         <v>76</v>
@@ -4116,13 +4076,13 @@
         <v>117193</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E28">
         <v>75</v>
@@ -4133,13 +4093,13 @@
         <v>117186</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E29">
         <v>74</v>
@@ -4150,13 +4110,13 @@
         <v>116953</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E30">
         <v>73</v>
@@ -4167,13 +4127,13 @@
         <v>116881</v>
       </c>
       <c r="B31" s="38" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E31" s="39">
         <v>72</v>
@@ -4436,13 +4396,13 @@
         <v>116797</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E32">
         <v>71</v>
@@ -4453,13 +4413,13 @@
         <v>116601</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E33">
         <v>70</v>
@@ -4470,13 +4430,13 @@
         <v>116448</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E34">
         <v>69</v>
@@ -4487,13 +4447,13 @@
         <v>116441</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C35" s="36" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E35" s="30">
         <v>68</v>
@@ -4756,13 +4716,13 @@
         <v>116197</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E36">
         <v>67</v>
@@ -4773,13 +4733,13 @@
         <v>115899</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D37" s="40" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E37" s="39">
         <v>66</v>
@@ -5042,13 +5002,13 @@
         <v>115777</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>51</v>
+        <v>229</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E38">
         <v>65</v>
@@ -5059,13 +5019,13 @@
         <v>115611</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E39">
         <v>64</v>
@@ -5076,13 +5036,13 @@
         <v>115610</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E40">
         <v>63</v>
@@ -5093,13 +5053,13 @@
         <v>115602</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E41">
         <v>62</v>
@@ -5110,13 +5070,13 @@
         <v>115390</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E42">
         <v>61</v>
@@ -5127,13 +5087,13 @@
         <v>115195</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E43">
         <v>60</v>
@@ -5144,13 +5104,13 @@
         <v>114961</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E44">
         <v>59</v>
@@ -5161,13 +5121,13 @@
         <v>114748</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E45">
         <v>58</v>
@@ -5178,13 +5138,13 @@
         <v>114517</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E46">
         <v>57</v>
@@ -5195,13 +5155,13 @@
         <v>114386</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E47">
         <v>56</v>
@@ -5212,13 +5172,13 @@
         <v>114152</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E48">
         <v>55</v>
@@ -5229,13 +5189,13 @@
         <v>113992</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E49">
         <v>54</v>
@@ -5246,13 +5206,13 @@
         <v>113584</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E50">
         <v>53</v>
@@ -5263,13 +5223,13 @@
         <v>113583</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E51">
         <v>52</v>
@@ -5280,13 +5240,13 @@
         <v>113181</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E52" s="25">
         <v>51</v>
@@ -5549,13 +5509,13 @@
         <v>112512</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E53">
         <v>50</v>
@@ -5566,13 +5526,13 @@
         <v>112478</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E54">
         <v>49</v>
@@ -5583,13 +5543,13 @@
         <v>112270</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E55">
         <v>48</v>
@@ -5600,13 +5560,13 @@
         <v>111848</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E56">
         <v>47</v>
@@ -5617,13 +5577,13 @@
         <v>111580</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E57">
         <v>46</v>
@@ -5634,13 +5594,13 @@
         <v>111220</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>32</v>
+        <v>230</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E58">
         <v>45</v>
@@ -5651,13 +5611,13 @@
         <v>110740</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E59">
         <v>44</v>
@@ -5668,13 +5628,13 @@
         <v>109367</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E60">
         <v>43</v>
@@ -5685,13 +5645,13 @@
         <v>109244</v>
       </c>
       <c r="B61" s="38" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E61" s="39">
         <v>42</v>
@@ -5954,13 +5914,13 @@
         <v>108950</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E62">
         <v>41</v>
@@ -5971,13 +5931,13 @@
         <v>108856</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>28</v>
+        <v>233</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E63">
         <v>40</v>
@@ -5988,13 +5948,13 @@
         <v>108855</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E64">
         <v>39</v>
@@ -6005,13 +5965,13 @@
         <v>108754</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E65">
         <v>38</v>
@@ -6022,13 +5982,13 @@
         <v>108617</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E66">
         <v>37</v>
@@ -6039,13 +5999,13 @@
         <v>108343</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E67" s="15">
         <v>36</v>
@@ -6308,13 +6268,13 @@
         <v>108342</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E68">
         <v>35</v>
@@ -6325,13 +6285,13 @@
         <v>107869</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E69">
         <v>34</v>
@@ -6342,13 +6302,13 @@
         <v>107491</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E70">
         <v>33</v>
@@ -6359,13 +6319,13 @@
         <v>106997</v>
       </c>
       <c r="B71" s="32" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C71" s="33" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D71" s="34" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E71" s="35">
         <v>32</v>
@@ -6628,13 +6588,13 @@
         <v>106993</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E72">
         <v>31</v>
@@ -6645,13 +6605,13 @@
         <v>106389</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E73">
         <v>30</v>
@@ -6662,13 +6622,13 @@
         <v>106388</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D74" s="19" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E74" s="20">
         <v>29</v>
@@ -6931,13 +6891,13 @@
         <v>106272</v>
       </c>
       <c r="B75" s="38" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E75" s="39">
         <v>28</v>
@@ -7200,13 +7160,13 @@
         <v>106042</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E76">
         <v>27</v>
@@ -7217,13 +7177,13 @@
         <v>105840</v>
       </c>
       <c r="B77" s="38" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E77" s="39">
         <v>26</v>
@@ -7486,13 +7446,13 @@
         <v>105655</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E78">
         <v>25</v>
@@ -7503,13 +7463,13 @@
         <v>104996</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E79">
         <v>24</v>
@@ -7520,13 +7480,13 @@
         <v>103293</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E80">
         <v>23</v>
@@ -7537,13 +7497,13 @@
         <v>102906</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E81">
         <v>22</v>
@@ -7554,13 +7514,13 @@
         <v>102687</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>14</v>
+        <v>232</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E82">
         <v>21</v>
@@ -7571,13 +7531,13 @@
         <v>102674</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C83" s="36" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E83" s="15">
         <v>20</v>
@@ -7840,13 +7800,13 @@
         <v>102289</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E84">
         <v>19</v>
@@ -7857,13 +7817,13 @@
         <v>102089</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E85">
         <v>18</v>
@@ -7874,13 +7834,13 @@
         <v>101596</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E86">
         <v>17</v>
@@ -7891,13 +7851,13 @@
         <v>101163</v>
       </c>
       <c r="B87" s="38" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E87" s="39">
         <v>16</v>
@@ -8160,13 +8120,13 @@
         <v>101162</v>
       </c>
       <c r="B88" s="32" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C88" s="33" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D88" s="34" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E88" s="35">
         <v>15</v>
@@ -8429,13 +8389,13 @@
         <v>100689</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E89">
         <v>14</v>
@@ -8446,13 +8406,13 @@
         <v>100680</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E90">
         <v>13</v>
@@ -8463,13 +8423,13 @@
         <v>100562</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E91">
         <v>12</v>
@@ -8480,13 +8440,13 @@
         <v>100010</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E92">
         <v>11</v>
@@ -8497,13 +8457,13 @@
         <v>99982</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E93">
         <v>10</v>
@@ -8514,13 +8474,13 @@
         <v>99716</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E94">
         <v>9</v>
@@ -8531,13 +8491,13 @@
         <v>99581</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>4</v>
+        <v>231</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E95">
         <v>8</v>
@@ -8548,13 +8508,13 @@
         <v>99480</v>
       </c>
       <c r="B96" s="38" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E96" s="39">
         <v>7</v>
@@ -8817,13 +8777,13 @@
         <v>98869</v>
       </c>
       <c r="B97" s="22" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C97" s="23" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D97" s="24" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E97" s="25">
         <v>6</v>
@@ -9086,13 +9046,13 @@
         <v>98578</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E98">
         <v>5</v>
@@ -9103,13 +9063,13 @@
         <v>98197</v>
       </c>
       <c r="B99" s="22" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C99" s="23" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D99" s="24" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E99" s="25">
         <v>4</v>
@@ -9372,13 +9332,13 @@
         <v>98078</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E100">
         <v>3</v>
@@ -9389,13 +9349,13 @@
         <v>98059</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E101">
         <v>2</v>
@@ -9406,13 +9366,13 @@
         <v>96024</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E102">
         <v>1</v>

</xml_diff>

<commit_message>
basic glm models and variable selection
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="15960" windowHeight="16380"/>
+    <workbookView xWindow="0" yWindow="165" windowWidth="15960" windowHeight="16320"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="237">
   <si>
     <r>
       <rPr>
@@ -1335,6 +1335,15 @@
   </si>
   <si>
     <t>Lots of people are around! Are you more likely to be right in the middle of things, or looking for your own quieter space?</t>
+  </si>
+  <si>
+    <t>Face validity</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -1501,7 +1510,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1624,6 +1633,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2842,18 +2854,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G102" sqref="G2:H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="75.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="92.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="22" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
-    <col min="6" max="257" width="9.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" style="1" customWidth="1"/>
+    <col min="7" max="257" width="9.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2872,6 +2885,9 @@
       <c r="E1" s="10" t="s">
         <v>182</v>
       </c>
+      <c r="F1" s="41" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="2" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
@@ -2889,6 +2905,17 @@
       <c r="E2">
         <v>101</v>
       </c>
+      <c r="F2" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G2" s="1" t="str">
+        <f>IF((F2="y"),B2, "")</f>
+        <v/>
+      </c>
+      <c r="H2" s="1" t="str">
+        <f>IF((F2="y"),E2, "")</f>
+        <v/>
+      </c>
     </row>
     <row r="3" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
@@ -2906,6 +2933,17 @@
       <c r="E3">
         <v>100</v>
       </c>
+      <c r="F3" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G3" s="1" t="str">
+        <f t="shared" ref="G3:G66" si="0">IF((F3="y"),B3, "")</f>
+        <v/>
+      </c>
+      <c r="H3" s="1" t="str">
+        <f t="shared" ref="H3:H66" si="1">IF((F3="y"),E3, "")</f>
+        <v/>
+      </c>
     </row>
     <row r="4" spans="1:257" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
@@ -2923,9 +2961,17 @@
       <c r="E4" s="20">
         <v>99</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
+      <c r="F4" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q123621</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="17"/>
@@ -3192,6 +3238,17 @@
       <c r="E5">
         <v>98</v>
       </c>
+      <c r="F5" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q123464</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
     </row>
     <row r="6" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
@@ -3209,6 +3266,17 @@
       <c r="E6">
         <v>97</v>
       </c>
+      <c r="F6" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q122771</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
     </row>
     <row r="7" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
@@ -3226,6 +3294,17 @@
       <c r="E7">
         <v>96</v>
       </c>
+      <c r="F7" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q122770</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
     </row>
     <row r="8" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
@@ -3243,6 +3322,17 @@
       <c r="E8">
         <v>95</v>
       </c>
+      <c r="F8" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="9" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
@@ -3260,6 +3350,17 @@
       <c r="E9">
         <v>94</v>
       </c>
+      <c r="F9" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="10" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
@@ -3277,6 +3378,17 @@
       <c r="E10">
         <v>93</v>
       </c>
+      <c r="F10" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="11" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
@@ -3294,6 +3406,17 @@
       <c r="E11">
         <v>92</v>
       </c>
+      <c r="F11" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="12" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
@@ -3311,6 +3434,17 @@
       <c r="E12">
         <v>91</v>
       </c>
+      <c r="F12" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="13" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
@@ -3328,6 +3462,17 @@
       <c r="E13">
         <v>90</v>
       </c>
+      <c r="F13" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="14" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
@@ -3345,6 +3490,17 @@
       <c r="E14">
         <v>89</v>
       </c>
+      <c r="F14" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q120650</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
     </row>
     <row r="15" spans="1:257" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="37">
@@ -3362,9 +3518,17 @@
       <c r="E15" s="39">
         <v>88</v>
       </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
+      <c r="F15" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q120472</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
       <c r="I15" s="38"/>
       <c r="J15" s="38"/>
       <c r="K15" s="38"/>
@@ -3631,9 +3795,17 @@
       <c r="E16" s="39">
         <v>87</v>
       </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
+      <c r="F16" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q120379</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
       <c r="I16" s="38"/>
       <c r="J16" s="38"/>
       <c r="K16" s="38"/>
@@ -3900,6 +4072,17 @@
       <c r="E17">
         <v>86</v>
       </c>
+      <c r="F17" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q120194</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
     </row>
     <row r="18" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
@@ -3917,6 +4100,17 @@
       <c r="E18">
         <v>85</v>
       </c>
+      <c r="F18" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q120014</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
     </row>
     <row r="19" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
@@ -3934,6 +4128,17 @@
       <c r="E19">
         <v>84</v>
       </c>
+      <c r="F19" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="20" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
@@ -3951,6 +4156,17 @@
       <c r="E20">
         <v>83</v>
       </c>
+      <c r="F20" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="21" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
@@ -3968,6 +4184,17 @@
       <c r="E21">
         <v>82</v>
       </c>
+      <c r="F21" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q119650</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
     </row>
     <row r="22" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
@@ -3985,6 +4212,17 @@
       <c r="E22">
         <v>81</v>
       </c>
+      <c r="F22" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q119334</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
     </row>
     <row r="23" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
@@ -4002,6 +4240,17 @@
       <c r="E23">
         <v>80</v>
       </c>
+      <c r="F23" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="24" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
@@ -4019,6 +4268,17 @@
       <c r="E24">
         <v>79</v>
       </c>
+      <c r="F24" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="25" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
@@ -4036,6 +4296,17 @@
       <c r="E25">
         <v>78</v>
       </c>
+      <c r="F25" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q118233</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
     </row>
     <row r="26" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
@@ -4053,6 +4324,17 @@
       <c r="E26">
         <v>77</v>
       </c>
+      <c r="F26" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q118232</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
     </row>
     <row r="27" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
@@ -4070,6 +4352,17 @@
       <c r="E27">
         <v>76</v>
       </c>
+      <c r="F27" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q118117</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="28" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
@@ -4087,6 +4380,17 @@
       <c r="E28">
         <v>75</v>
       </c>
+      <c r="F28" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q117193</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
     </row>
     <row r="29" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
@@ -4104,6 +4408,17 @@
       <c r="E29">
         <v>74</v>
       </c>
+      <c r="F29" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="30" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
@@ -4121,6 +4436,17 @@
       <c r="E30">
         <v>73</v>
       </c>
+      <c r="F30" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q116953</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
     </row>
     <row r="31" spans="1:257" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="37">
@@ -4138,9 +4464,17 @@
       <c r="E31" s="39">
         <v>72</v>
       </c>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
+      <c r="F31" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q116881</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
       <c r="I31" s="38"/>
       <c r="J31" s="38"/>
       <c r="K31" s="38"/>
@@ -4407,6 +4741,17 @@
       <c r="E32">
         <v>71</v>
       </c>
+      <c r="F32" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H32" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="33" spans="1:257" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
@@ -4424,6 +4769,17 @@
       <c r="E33">
         <v>70</v>
       </c>
+      <c r="F33" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q116601</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
     </row>
     <row r="34" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
@@ -4441,6 +4797,17 @@
       <c r="E34">
         <v>69</v>
       </c>
+      <c r="F34" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H34" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="35" spans="1:257" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="26">
@@ -4458,9 +4825,17 @@
       <c r="E35" s="30">
         <v>68</v>
       </c>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
+      <c r="F35" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="G35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H35" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="I35" s="27"/>
       <c r="J35" s="27"/>
       <c r="K35" s="27"/>
@@ -4727,6 +5102,17 @@
       <c r="E36">
         <v>67</v>
       </c>
+      <c r="F36" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H36" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="37" spans="1:257" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="37">
@@ -4744,9 +5130,17 @@
       <c r="E37" s="39">
         <v>66</v>
       </c>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
+      <c r="F37" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q115899</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
       <c r="I37" s="38"/>
       <c r="J37" s="38"/>
       <c r="K37" s="38"/>
@@ -5013,6 +5407,17 @@
       <c r="E38">
         <v>65</v>
       </c>
+      <c r="F38" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H38" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="39" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
@@ -5030,6 +5435,17 @@
       <c r="E39">
         <v>64</v>
       </c>
+      <c r="F39" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q115611</v>
+      </c>
+      <c r="H39" s="1">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
     </row>
     <row r="40" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
@@ -5047,6 +5463,17 @@
       <c r="E40">
         <v>63</v>
       </c>
+      <c r="F40" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q115610</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
     </row>
     <row r="41" spans="1:257" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
@@ -5064,6 +5491,17 @@
       <c r="E41">
         <v>62</v>
       </c>
+      <c r="F41" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q115602</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
     </row>
     <row r="42" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
@@ -5081,6 +5519,17 @@
       <c r="E42">
         <v>61</v>
       </c>
+      <c r="F42" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H42" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="43" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
@@ -5098,6 +5547,17 @@
       <c r="E43">
         <v>60</v>
       </c>
+      <c r="F43" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q115195</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="44" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
@@ -5115,6 +5575,17 @@
       <c r="E44">
         <v>59</v>
       </c>
+      <c r="F44" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q114961</v>
+      </c>
+      <c r="H44" s="1">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
     </row>
     <row r="45" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
@@ -5132,6 +5603,17 @@
       <c r="E45">
         <v>58</v>
       </c>
+      <c r="F45" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q114748</v>
+      </c>
+      <c r="H45" s="1">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
     </row>
     <row r="46" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
@@ -5149,6 +5631,17 @@
       <c r="E46">
         <v>57</v>
       </c>
+      <c r="F46" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H46" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="47" spans="1:257" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
@@ -5166,6 +5659,17 @@
       <c r="E47">
         <v>56</v>
       </c>
+      <c r="F47" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H47" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="48" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
@@ -5183,6 +5687,17 @@
       <c r="E48">
         <v>55</v>
       </c>
+      <c r="F48" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q114152</v>
+      </c>
+      <c r="H48" s="1">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
     </row>
     <row r="49" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
@@ -5200,6 +5715,17 @@
       <c r="E49">
         <v>54</v>
       </c>
+      <c r="F49" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q113992</v>
+      </c>
+      <c r="H49" s="1">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
     </row>
     <row r="50" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
@@ -5217,6 +5743,17 @@
       <c r="E50">
         <v>53</v>
       </c>
+      <c r="F50" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H50" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="51" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
@@ -5234,6 +5771,17 @@
       <c r="E51">
         <v>52</v>
       </c>
+      <c r="F51" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q113583</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="52" spans="1:257" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="21">
@@ -5251,9 +5799,17 @@
       <c r="E52" s="25">
         <v>51</v>
       </c>
-      <c r="F52" s="22"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="22"/>
+      <c r="F52" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="G52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q113181</v>
+      </c>
+      <c r="H52" s="1">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
       <c r="I52" s="22"/>
       <c r="J52" s="22"/>
       <c r="K52" s="22"/>
@@ -5520,6 +6076,17 @@
       <c r="E53">
         <v>50</v>
       </c>
+      <c r="F53" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H53" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="54" spans="1:257" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
@@ -5537,6 +6104,17 @@
       <c r="E54">
         <v>49</v>
       </c>
+      <c r="F54" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H54" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="55" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
@@ -5554,6 +6132,17 @@
       <c r="E55">
         <v>48</v>
       </c>
+      <c r="F55" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H55" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="56" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
@@ -5571,6 +6160,17 @@
       <c r="E56">
         <v>47</v>
       </c>
+      <c r="F56" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q111848</v>
+      </c>
+      <c r="H56" s="1">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
     </row>
     <row r="57" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
@@ -5588,6 +6188,17 @@
       <c r="E57">
         <v>46</v>
       </c>
+      <c r="F57" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q111580</v>
+      </c>
+      <c r="H57" s="1">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="58" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
@@ -5605,6 +6216,17 @@
       <c r="E58">
         <v>45</v>
       </c>
+      <c r="F58" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H58" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="59" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5">
@@ -5622,6 +6244,17 @@
       <c r="E59">
         <v>44</v>
       </c>
+      <c r="F59" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q110740</v>
+      </c>
+      <c r="H59" s="1">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="60" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
@@ -5639,6 +6272,17 @@
       <c r="E60">
         <v>43</v>
       </c>
+      <c r="F60" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q109367</v>
+      </c>
+      <c r="H60" s="1">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="61" spans="1:257" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="37">
@@ -5656,9 +6300,17 @@
       <c r="E61" s="39">
         <v>42</v>
       </c>
-      <c r="F61" s="38"/>
-      <c r="G61" s="38"/>
-      <c r="H61" s="38"/>
+      <c r="F61" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G61" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q109244</v>
+      </c>
+      <c r="H61" s="1">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
       <c r="I61" s="38"/>
       <c r="J61" s="38"/>
       <c r="K61" s="38"/>
@@ -5925,6 +6577,17 @@
       <c r="E62">
         <v>41</v>
       </c>
+      <c r="F62" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G62" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H62" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="63" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
@@ -5942,6 +6605,17 @@
       <c r="E63">
         <v>40</v>
       </c>
+      <c r="F63" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q108856</v>
+      </c>
+      <c r="H63" s="1">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="64" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
@@ -5959,6 +6633,17 @@
       <c r="E64">
         <v>39</v>
       </c>
+      <c r="F64" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q108855</v>
+      </c>
+      <c r="H64" s="1">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
     </row>
     <row r="65" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
@@ -5976,6 +6661,17 @@
       <c r="E65">
         <v>38</v>
       </c>
+      <c r="F65" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G65" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q108754</v>
+      </c>
+      <c r="H65" s="1">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="66" spans="1:257" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="5">
@@ -5993,6 +6689,17 @@
       <c r="E66">
         <v>37</v>
       </c>
+      <c r="F66" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G66" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Q108617</v>
+      </c>
+      <c r="H66" s="1">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="67" spans="1:257" s="15" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="11">
@@ -6010,9 +6717,17 @@
       <c r="E67" s="15">
         <v>36</v>
       </c>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="12"/>
+      <c r="F67" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="G67" s="1" t="str">
+        <f t="shared" ref="G67:G102" si="2">IF((F67="y"),B67, "")</f>
+        <v>Q108343</v>
+      </c>
+      <c r="H67" s="1">
+        <f t="shared" ref="H67:H102" si="3">IF((F67="y"),E67, "")</f>
+        <v>36</v>
+      </c>
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
       <c r="K67" s="12"/>
@@ -6279,6 +6994,17 @@
       <c r="E68">
         <v>35</v>
       </c>
+      <c r="F68" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G68" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Q108342</v>
+      </c>
+      <c r="H68" s="1">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="69" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
@@ -6296,6 +7022,17 @@
       <c r="E69">
         <v>34</v>
       </c>
+      <c r="F69" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G69" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H69" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="70" spans="1:257" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="5">
@@ -6313,6 +7050,17 @@
       <c r="E70">
         <v>33</v>
       </c>
+      <c r="F70" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G70" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H70" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="71" spans="1:257" s="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="31">
@@ -6330,9 +7078,17 @@
       <c r="E71" s="35">
         <v>32</v>
       </c>
-      <c r="F71" s="32"/>
-      <c r="G71" s="32"/>
-      <c r="H71" s="32"/>
+      <c r="F71" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="G71" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H71" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="I71" s="32"/>
       <c r="J71" s="32"/>
       <c r="K71" s="32"/>
@@ -6599,6 +7355,17 @@
       <c r="E72">
         <v>31</v>
       </c>
+      <c r="F72" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G72" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H72" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="73" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="5">
@@ -6616,6 +7383,17 @@
       <c r="E73">
         <v>30</v>
       </c>
+      <c r="F73" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G73" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H73" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="74" spans="1:257" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="16">
@@ -6633,9 +7411,17 @@
       <c r="E74" s="20">
         <v>29</v>
       </c>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
+      <c r="F74" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="G74" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Q106388</v>
+      </c>
+      <c r="H74" s="1">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
       <c r="I74" s="17"/>
       <c r="J74" s="17"/>
       <c r="K74" s="17"/>
@@ -6902,9 +7688,17 @@
       <c r="E75" s="39">
         <v>28</v>
       </c>
-      <c r="F75" s="38"/>
-      <c r="G75" s="38"/>
-      <c r="H75" s="38"/>
+      <c r="F75" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G75" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Q106272</v>
+      </c>
+      <c r="H75" s="1">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
       <c r="I75" s="38"/>
       <c r="J75" s="38"/>
       <c r="K75" s="38"/>
@@ -7171,6 +7965,17 @@
       <c r="E76">
         <v>27</v>
       </c>
+      <c r="F76" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G76" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Q106042</v>
+      </c>
+      <c r="H76" s="1">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="77" spans="1:257" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="37">
@@ -7188,9 +7993,17 @@
       <c r="E77" s="39">
         <v>26</v>
       </c>
-      <c r="F77" s="38"/>
-      <c r="G77" s="38"/>
-      <c r="H77" s="38"/>
+      <c r="F77" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G77" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Q105840</v>
+      </c>
+      <c r="H77" s="1">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
       <c r="I77" s="38"/>
       <c r="J77" s="38"/>
       <c r="K77" s="38"/>
@@ -7457,6 +8270,17 @@
       <c r="E78">
         <v>25</v>
       </c>
+      <c r="F78" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G78" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H78" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="79" spans="1:257" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="5">
@@ -7474,6 +8298,17 @@
       <c r="E79">
         <v>24</v>
       </c>
+      <c r="F79" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G79" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H79" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="80" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="5">
@@ -7491,6 +8326,17 @@
       <c r="E80">
         <v>23</v>
       </c>
+      <c r="F80" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G80" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H80" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="81" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="5">
@@ -7508,6 +8354,17 @@
       <c r="E81">
         <v>22</v>
       </c>
+      <c r="F81" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G81" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H81" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="82" spans="1:257" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="5">
@@ -7525,6 +8382,17 @@
       <c r="E82">
         <v>21</v>
       </c>
+      <c r="F82" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G82" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H82" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="83" spans="1:257" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11">
@@ -7542,9 +8410,17 @@
       <c r="E83" s="15">
         <v>20</v>
       </c>
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="12"/>
+      <c r="F83" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="G83" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Q102674</v>
+      </c>
+      <c r="H83" s="1">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="I83" s="12"/>
       <c r="J83" s="12"/>
       <c r="K83" s="12"/>
@@ -7811,6 +8687,17 @@
       <c r="E84">
         <v>19</v>
       </c>
+      <c r="F84" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G84" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H84" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="85" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="5">
@@ -7828,6 +8715,17 @@
       <c r="E85">
         <v>18</v>
       </c>
+      <c r="F85" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G85" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Q102089</v>
+      </c>
+      <c r="H85" s="1">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="86" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="5">
@@ -7845,6 +8743,17 @@
       <c r="E86">
         <v>17</v>
       </c>
+      <c r="F86" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G86" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H86" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="87" spans="1:257" s="39" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="37">
@@ -7862,9 +8771,17 @@
       <c r="E87" s="39">
         <v>16</v>
       </c>
-      <c r="F87" s="38"/>
-      <c r="G87" s="38"/>
-      <c r="H87" s="38"/>
+      <c r="F87" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G87" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Q101163</v>
+      </c>
+      <c r="H87" s="1">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
       <c r="I87" s="38"/>
       <c r="J87" s="38"/>
       <c r="K87" s="38"/>
@@ -8131,9 +9048,17 @@
       <c r="E88" s="35">
         <v>15</v>
       </c>
-      <c r="F88" s="32"/>
-      <c r="G88" s="32"/>
-      <c r="H88" s="32"/>
+      <c r="F88" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="G88" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Q101162</v>
+      </c>
+      <c r="H88" s="1">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
       <c r="I88" s="32"/>
       <c r="J88" s="32"/>
       <c r="K88" s="32"/>
@@ -8400,6 +9325,17 @@
       <c r="E89">
         <v>14</v>
       </c>
+      <c r="F89" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G89" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H89" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="90" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="5">
@@ -8417,6 +9353,17 @@
       <c r="E90">
         <v>13</v>
       </c>
+      <c r="F90" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G90" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H90" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="91" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="5">
@@ -8434,6 +9381,17 @@
       <c r="E91">
         <v>12</v>
       </c>
+      <c r="F91" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G91" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Q100562</v>
+      </c>
+      <c r="H91" s="1">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="92" spans="1:257" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="5">
@@ -8451,6 +9409,17 @@
       <c r="E92">
         <v>11</v>
       </c>
+      <c r="F92" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G92" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H92" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="93" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="5">
@@ -8468,6 +9437,17 @@
       <c r="E93">
         <v>10</v>
       </c>
+      <c r="F93" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G93" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H93" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="94" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="5">
@@ -8485,6 +9465,17 @@
       <c r="E94">
         <v>9</v>
       </c>
+      <c r="F94" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G94" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Q99716</v>
+      </c>
+      <c r="H94" s="1">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="95" spans="1:257" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="5">
@@ -8502,6 +9493,17 @@
       <c r="E95">
         <v>8</v>
       </c>
+      <c r="F95" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G95" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H95" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="96" spans="1:257" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="37">
@@ -8519,9 +9521,17 @@
       <c r="E96" s="39">
         <v>7</v>
       </c>
-      <c r="F96" s="38"/>
-      <c r="G96" s="38"/>
-      <c r="H96" s="38"/>
+      <c r="F96" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="G96" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Q99480</v>
+      </c>
+      <c r="H96" s="1">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
       <c r="I96" s="38"/>
       <c r="J96" s="38"/>
       <c r="K96" s="38"/>
@@ -8788,9 +9798,17 @@
       <c r="E97" s="25">
         <v>6</v>
       </c>
-      <c r="F97" s="22"/>
-      <c r="G97" s="22"/>
-      <c r="H97" s="22"/>
+      <c r="F97" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="G97" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Q98869</v>
+      </c>
+      <c r="H97" s="1">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
       <c r="I97" s="22"/>
       <c r="J97" s="22"/>
       <c r="K97" s="22"/>
@@ -9057,6 +10075,17 @@
       <c r="E98">
         <v>5</v>
       </c>
+      <c r="F98" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="G98" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Q98578</v>
+      </c>
+      <c r="H98" s="1">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="99" spans="1:257" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="21">
@@ -9074,9 +10103,17 @@
       <c r="E99" s="25">
         <v>4</v>
       </c>
-      <c r="F99" s="22"/>
-      <c r="G99" s="22"/>
-      <c r="H99" s="22"/>
+      <c r="F99" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="G99" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H99" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="I99" s="22"/>
       <c r="J99" s="22"/>
       <c r="K99" s="22"/>
@@ -9343,6 +10380,17 @@
       <c r="E100">
         <v>3</v>
       </c>
+      <c r="F100" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G100" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H100" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="101" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="5">
@@ -9360,6 +10408,17 @@
       <c r="E101">
         <v>2</v>
       </c>
+      <c r="F101" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G101" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H101" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="102" spans="1:257" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="5">
@@ -9376,6 +10435,17 @@
       </c>
       <c r="E102">
         <v>1</v>
+      </c>
+      <c r="F102" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="G102" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H102" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>